<commit_message>
ExpectimaxN for partial states
- new ExpectimaxN version for imperfect-information games
- StateObservation, StateObserverKuhnPoker: added isImperfectInformationGame and completePartialState(p,root)
- new tests in TreeKuhnPokerTest
</commit_message>
<xml_diff>
--- a/resources/ASimpleGameWhereTDLearningFails.xlsx
+++ b/resources/ASimpleGameWhereTDLearningFails.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wolfgang\Documents\GitHub\GBG\myDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wolfgang\Documents\GitHub\GBG\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B95770-F308-48F5-A5D8-B86FBA2FE5C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3060E49-BEF1-4293-99CA-F78BDA7BEBCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8592" xr2:uid="{2C07B2E9-67BD-491D-8D63-935BCA8F6CEC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>HIT</t>
   </si>
@@ -91,6 +91,27 @@
   </si>
   <si>
     <t>This is because Q(s,a) should approach expected reward (cols D and E), if learning rate is sufficiently small</t>
+  </si>
+  <si>
+    <t>Optimal policy:</t>
+  </si>
+  <si>
+    <t>Select HIT, if expec. reward(HIT) is higher than expec. reward(STAND)</t>
+  </si>
+  <si>
+    <t>with</t>
+  </si>
+  <si>
+    <t>C = current sum</t>
+  </si>
+  <si>
+    <t>A = new card \in {1,…,9-C}</t>
+  </si>
+  <si>
+    <t>Expec. Reward(HIT): (C + E[A])*P[A] + 0*P[NOT A]</t>
+  </si>
+  <si>
+    <t>It turns out (see columns D and E) that we should select HIT only if C \in {1,2,3}</t>
   </si>
 </sst>
 </file>
@@ -98,7 +119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -181,15 +202,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -504,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43D1659-4079-4B93-AC42-001001C8702D}">
-  <dimension ref="C2:Q25"/>
+  <dimension ref="C2:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,26 +567,26 @@
       </c>
     </row>
     <row r="8" spans="3:17" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="G8" s="5" t="s">
+      <c r="E8" s="8"/>
+      <c r="G8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5" t="s">
+      <c r="H8" s="8"/>
+      <c r="I8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="M8" s="6" t="s">
+      <c r="J8" s="8"/>
+      <c r="M8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="6"/>
-      <c r="P8" s="6" t="s">
+      <c r="N8" s="9"/>
+      <c r="P8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="Q8" s="6"/>
+      <c r="Q8" s="9"/>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
@@ -600,7 +621,7 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <f>(C10+AVERAGE(C10:C17))*COUNT(C10:C17)/9</f>
         <v>4.8888888888888893</v>
       </c>
@@ -642,7 +663,7 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <f>(C11+AVERAGE(C10:C16))*COUNT(C10:C16)/9</f>
         <v>4.666666666666667</v>
       </c>
@@ -684,7 +705,7 @@
       <c r="C12">
         <v>3</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <f>(C12+AVERAGE(C10:C15))*COUNT(C10:C15)/9</f>
         <v>4.333333333333333</v>
       </c>
@@ -730,7 +751,7 @@
         <f>(C13+AVERAGE(C10:C14))*COUNT(C10:C14)/9</f>
         <v>3.8888888888888888</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>4</v>
       </c>
       <c r="F13">
@@ -772,7 +793,7 @@
         <f>(C14+AVERAGE(C10:C13))*COUNT(C10:C13)/9</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="5">
         <v>5</v>
       </c>
       <c r="F14">
@@ -814,7 +835,7 @@
         <f>(C15+AVERAGE(C10:C12))*COUNT(C10:C12)/9</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="5">
         <v>6</v>
       </c>
       <c r="F15">
@@ -856,7 +877,7 @@
         <f>(C16+AVERAGE(C10:C11))*COUNT(C10:C11)/9</f>
         <v>1.8888888888888888</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="5">
         <v>7</v>
       </c>
       <c r="F16">
@@ -898,7 +919,7 @@
         <f>(C17+AVERAGE(C10:C10))*COUNT(C10:C10)/9</f>
         <v>1</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <v>8</v>
       </c>
       <c r="F17">
@@ -939,7 +960,7 @@
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="5">
         <v>9</v>
       </c>
       <c r="F18">
@@ -974,7 +995,7 @@
       </c>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I20" s="3"/>
@@ -986,14 +1007,14 @@
         <v>5.2880658436213999</v>
       </c>
       <c r="L20" s="1"/>
-      <c r="M20" s="7" t="s">
+      <c r="M20" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N20" s="5">
         <f>AVERAGE(N10:N18)</f>
         <v>5.8765432098765427</v>
       </c>
-      <c r="P20" s="8">
+      <c r="P20" s="6">
         <f>AVERAGE(P10:P18)</f>
         <v>3.9814814814814818</v>
       </c>
@@ -1017,10 +1038,10 @@
         <f>AVERAGE(I10:I12,J13:J17)</f>
         <v>0.70833333333333326</v>
       </c>
-      <c r="N22" s="9">
-        <v>1</v>
-      </c>
-      <c r="P22" s="8">
+      <c r="N22" s="7">
+        <v>1</v>
+      </c>
+      <c r="P22" s="6">
         <v>0.5</v>
       </c>
     </row>
@@ -1032,6 +1053,39 @@
     <row r="25" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>